<commit_message>
add: github workflow and 2025国赛资料
</commit_message>
<xml_diff>
--- a/历年赛题/国赛/分类.xlsx
+++ b/历年赛题/国赛/分类.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\robot\project\NUEDC_Topic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDLZ\Desktop\myOpenSource\nwpu-nuedc\历年赛题\国赛\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6767AD6-2387-47A9-9929-825371389C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB156A1-6CCF-4617-B057-442FFCD9CB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>A_简易数控直流电源</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -544,6 +544,32 @@
     <t>E题_三子棋游戏装置
 F题_磁悬浮实验装置
 H题_自动行驶小车</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>D_简易以太网双绞线测试仪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_简易自动接收机</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>A_能量回馈的变流器负载试验装置
+B_单相有源电力滤波实验装置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>H_野生动物巡查系统</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G_电路模型探究装置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_简易自行瞄准装置
+C_基于单目视觉的目标物测量装置</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1171,31 +1197,31 @@
     <cellStyle name="60% - 着色 4" xfId="32" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - 着色 5" xfId="36" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - 着色 6" xfId="40" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="41" xr:uid="{51E31E59-FA2F-42BD-96AA-AD5B2CCEA10D}"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="41" xr:uid="{51E31E59-FA2F-42BD-96AA-AD5B2CCEA10D}"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="汇总" xfId="16" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="15" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="注释 2" xfId="42" xr:uid="{73F7F688-72A0-477D-808D-79FC07E2099C}"/>
     <cellStyle name="着色 1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="着色 2" xfId="21" builtinId="33" customBuiltin="1"/>
     <cellStyle name="着色 3" xfId="25" builtinId="37" customBuiltin="1"/>
     <cellStyle name="着色 4" xfId="29" builtinId="41" customBuiltin="1"/>
     <cellStyle name="着色 5" xfId="33" builtinId="45" customBuiltin="1"/>
     <cellStyle name="着色 6" xfId="37" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释 2" xfId="42" xr:uid="{73F7F688-72A0-477D-808D-79FC07E2099C}"/>
+    <cellStyle name="解释性文本" xfId="15" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1474,22 +1500,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="30.58203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="1" customWidth="1"/>
-    <col min="2" max="5" width="30.625" style="1"/>
-    <col min="6" max="6" width="30.875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.625" style="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="30.58203125" style="1"/>
+    <col min="6" max="6" width="30.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1522,7 +1548,7 @@
       <c r="M1"/>
       <c r="N1"/>
     </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1994</v>
       </c>
@@ -1533,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1995</v>
       </c>
@@ -1544,7 +1570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1997</v>
       </c>
@@ -1561,7 +1587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1999</v>
       </c>
@@ -1578,7 +1604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2001</v>
       </c>
@@ -1595,7 +1621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2003</v>
       </c>
@@ -1612,7 +1638,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2005</v>
       </c>
@@ -1629,7 +1655,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2007</v>
       </c>
@@ -1652,7 +1678,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2009</v>
       </c>
@@ -1678,7 +1704,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
@@ -1698,7 +1724,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2013</v>
       </c>
@@ -1721,7 +1747,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2015</v>
       </c>
@@ -1747,7 +1773,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2017</v>
       </c>
@@ -1773,7 +1799,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2018</v>
       </c>
@@ -1803,7 +1829,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2019</v>
       </c>
@@ -1827,7 +1853,7 @@
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2020</v>
       </c>
@@ -1850,7 +1876,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2021</v>
       </c>
@@ -1880,7 +1906,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2022</v>
       </c>
@@ -1907,7 +1933,7 @@
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -1930,7 +1956,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2024</v>
       </c>
@@ -1951,6 +1977,29 @@
       </c>
       <c r="H21" s="1" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>